<commit_message>
Test Data from Odometer Correction
</commit_message>
<xml_diff>
--- a/Lab2/OdometerCorrectionData.xlsx
+++ b/Lab2/OdometerCorrectionData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\McGill\FALL 2019\ECSE 211 Design Principles and Methods\Labs\Lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA55CC6B-178C-4C19-9DEE-84D343F0E6E3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D955D467-F1BF-4DE8-BCC1-48F3671045A8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9D9E9656-AEC8-42A7-BF30-62317BCFE20A}"/>
   </bookViews>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A2EC221-4D54-4E34-BF3F-FAC6F442AAA6}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="139" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,7 +583,7 @@
         <v>17.3</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f>SQRT((C10-A10)^2+(D10-B10)^2)</f>
         <v>1.8208239892971525</v>
       </c>
     </row>
@@ -600,10 +600,6 @@
       <c r="D11">
         <v>21</v>
       </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>2.0890428430264412</v>
-      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -611,11 +607,155 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12.88</v>
+      </c>
+      <c r="B14">
+        <v>16.5</v>
+      </c>
       <c r="C14">
-        <v>14.2</v>
+        <v>12.1</v>
       </c>
       <c r="D14">
-        <v>19.100000000000001</v>
+        <v>17.899999999999999</v>
+      </c>
+      <c r="E14">
+        <f>SQRT((C14-A14)^2+(D14-B14)^2)</f>
+        <v>1.6026228502052495</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>11.31</v>
+      </c>
+      <c r="B15">
+        <v>18.850000000000001</v>
+      </c>
+      <c r="C15">
+        <v>11.7</v>
+      </c>
+      <c r="D15">
+        <v>21.1</v>
+      </c>
+      <c r="E15">
+        <f>SQRT((C15-A15)^2+(D15-B15)^2)</f>
+        <v>2.2835498680782074</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>12.05</v>
+      </c>
+      <c r="B16">
+        <v>19.850000000000001</v>
+      </c>
+      <c r="C16">
+        <v>12.5</v>
+      </c>
+      <c r="D16">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>12.88</v>
+      </c>
+      <c r="B17">
+        <v>18.329999999999998</v>
+      </c>
+      <c r="C17">
+        <v>13.3</v>
+      </c>
+      <c r="D17">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>11.74</v>
+      </c>
+      <c r="B18">
+        <v>17.71</v>
+      </c>
+      <c r="C18">
+        <v>11.8</v>
+      </c>
+      <c r="D18">
+        <v>19.8</v>
+      </c>
+      <c r="E18">
+        <f>SQRT((C18-A18)^2+(D18-B18)^2)</f>
+        <v>2.0908610666421619</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>11.56</v>
+      </c>
+      <c r="B19">
+        <v>19.329999999999998</v>
+      </c>
+      <c r="C19">
+        <v>11.75</v>
+      </c>
+      <c r="D19">
+        <v>20.399999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>10.220000000000001</v>
+      </c>
+      <c r="B20">
+        <v>15.31</v>
+      </c>
+      <c r="C20">
+        <v>10.3</v>
+      </c>
+      <c r="D20">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>13.41</v>
+      </c>
+      <c r="B21">
+        <v>18.670000000000002</v>
+      </c>
+      <c r="C21">
+        <v>13.1</v>
+      </c>
+      <c r="D21">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>10.16</v>
+      </c>
+      <c r="B22">
+        <v>18.940000000000001</v>
+      </c>
+      <c r="C22">
+        <v>10.1</v>
+      </c>
+      <c r="D22">
+        <v>17.600000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>10.75</v>
+      </c>
+      <c r="B23">
+        <v>17.04</v>
+      </c>
+      <c r="C23">
+        <v>10.6</v>
+      </c>
+      <c r="D23">
+        <v>15.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>